<commit_message>
Update Rank the Star Wars Films (Responses).xlsx
</commit_message>
<xml_diff>
--- a/SQL and R/Rank the Star Wars Films (Responses).xlsx
+++ b/SQL and R/Rank the Star Wars Films (Responses).xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nycdoe\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nycdoe\Documents\CUNY\DATA607\Assignments\SQL and R\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7190"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7190" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="movies" sheetId="1" r:id="rId1"/>
@@ -38,9 +38,6 @@
     <t>agarcia@energytechhs.org</t>
   </si>
   <si>
-    <t>userid</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -81,6 +78,9 @@
   </si>
   <si>
     <t>Episode VII: The Force Awakens</t>
+  </si>
+  <si>
+    <t>nameid</t>
   </si>
 </sst>
 </file>
@@ -348,9 +348,9 @@
   </sheetPr>
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomLeft" sqref="A1:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -362,10 +362,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
         <v>7</v>
-      </c>
-      <c r="B1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -373,7 +373,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -381,7 +381,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -389,7 +389,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -397,7 +397,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -405,7 +405,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -413,7 +413,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -421,7 +421,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -429,7 +429,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -437,7 +437,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -450,23 +450,23 @@
   <dimension ref="A1:M46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
         <v>16</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -1158,8 +1158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1169,10 +1169,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>